<commit_message>
new examples of students
</commit_message>
<xml_diff>
--- a/student_data_in_v2.xlsx
+++ b/student_data_in_v2.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -357,10 +357,10 @@
   <dimension ref="A1:BY2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="BY2" activeCellId="0" sqref="AY2:BY2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -595,236 +595,155 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>120045</v>
-      </c>
-      <c r="B2" s="1" t="n">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>119919</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="X2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="V2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="W2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="X2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="Z2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AC2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AE2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AF2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AG2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AI2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AK2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AL2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AM2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AN2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AO2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AP2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AQ2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AR2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AS2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AT2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AU2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AV2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AW2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AX2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AY2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AZ2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BA2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BB2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BC2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="BD2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="BE2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BF2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BG2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BH2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BI2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BJ2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BK2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BL2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BM2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BN2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BO2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BP2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BQ2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BR2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BS2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BT2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BU2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BV2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BW2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BX2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BY2" s="1" t="n">
+      <c r="Y2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AX2" s="0" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>